<commit_message>
Vendor Advisory and Patch links
</commit_message>
<xml_diff>
--- a/keywords_demo.xlsx
+++ b/keywords_demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Clones Personal\CVE-Crawler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-Clones\CVEGuard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C9FC07-496A-446B-B670-BD800CED5626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126260BE-9930-4F18-B621-01151BD19847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Google</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
   </si>
 </sst>
 </file>
@@ -372,32 +375,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -407,27 +413,32 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>